<commit_message>
cs4354 daughterboard fix, axo-preenfm2 analog input now working
</commit_message>
<xml_diff>
--- a/axo-on-preenfm2-pinout.xlsx
+++ b/axo-on-preenfm2-pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="129">
   <si>
     <t xml:space="preserve">Preen405 PIN</t>
   </si>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">LCD_DB6</t>
   </si>
   <si>
-    <t xml:space="preserve">I2S3_WS</t>
+    <t xml:space="preserve">now I2S3_WS</t>
   </si>
   <si>
     <t xml:space="preserve">PA5</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">assignable (SPI3_SCK)</t>
   </si>
   <si>
-    <t xml:space="preserve">I2S3_CK</t>
+    <t xml:space="preserve">now I2S3_CK</t>
   </si>
   <si>
     <t xml:space="preserve">Was: MCP4922 SCK</t>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">assignable (SPI3_MISO)</t>
   </si>
   <si>
-    <t xml:space="preserve">Was: MCP4922-1 CS</t>
+    <t xml:space="preserve">Was: MCP4922 CS1</t>
   </si>
   <si>
     <t xml:space="preserve">PB5</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">Switch 1 (PB5/BOOT0)</t>
   </si>
   <si>
-    <t xml:space="preserve">I2S3_SD</t>
+    <t xml:space="preserve">now I2S3_SD</t>
   </si>
   <si>
     <t xml:space="preserve">Was: MCP4922 MO</t>
@@ -265,7 +265,7 @@
     <t xml:space="preserve">assignable (I2C1_SDA)</t>
   </si>
   <si>
-    <t xml:space="preserve">Was: MCP4922-2 CS</t>
+    <t xml:space="preserve">Was: MCP4922 CS2</t>
   </si>
   <si>
     <t xml:space="preserve">PC0</t>
@@ -274,19 +274,25 @@
     <t xml:space="preserve">assignable(AIN1)</t>
   </si>
   <si>
+    <t xml:space="preserve">gate in</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC1</t>
   </si>
   <si>
     <t xml:space="preserve">assignable(AIN2)</t>
   </si>
   <si>
+    <t xml:space="preserve">CV in</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC10</t>
   </si>
   <si>
     <t xml:space="preserve">SDIO_D2</t>
   </si>
   <si>
-    <t xml:space="preserve">SD card</t>
+    <t xml:space="preserve">SD card D2</t>
   </si>
   <si>
     <t xml:space="preserve">PC11</t>
@@ -295,6 +301,9 @@
     <t xml:space="preserve">SDIO_D3</t>
   </si>
   <si>
+    <t xml:space="preserve">SD card D3</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC12</t>
   </si>
   <si>
@@ -304,6 +313,9 @@
     <t xml:space="preserve">SDIO_CK</t>
   </si>
   <si>
+    <t xml:space="preserve">SD card CK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Was: MCP4922 LDAC</t>
   </si>
   <si>
@@ -334,7 +346,7 @@
     <t xml:space="preserve">PC7</t>
   </si>
   <si>
-    <t xml:space="preserve">I2S3_MCK</t>
+    <t xml:space="preserve">now I2S3_MCK</t>
   </si>
   <si>
     <t xml:space="preserve">PC8</t>
@@ -343,12 +355,18 @@
     <t xml:space="preserve">SDIO_D0</t>
   </si>
   <si>
+    <t xml:space="preserve">SD card D0</t>
+  </si>
+  <si>
     <t xml:space="preserve">PD2</t>
   </si>
   <si>
     <t xml:space="preserve">SDIO_CMD</t>
   </si>
   <si>
+    <t xml:space="preserve">SD card CMD</t>
+  </si>
+  <si>
     <t xml:space="preserve">*41</t>
   </si>
   <si>
@@ -359,6 +377,9 @@
   </si>
   <si>
     <t xml:space="preserve">SDIO_D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD card D1</t>
   </si>
   <si>
     <t xml:space="preserve">D2</t>
@@ -445,7 +466,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,12 +489,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE0EFD4"/>
         <bgColor rgb="FFEEEEEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF87D1D1"/>
-        <bgColor rgb="FFC2E0AE"/>
       </patternFill>
     </fill>
     <fill>
@@ -542,7 +557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -595,10 +610,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -611,59 +622,47 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -714,7 +713,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFE0EFD4"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF87D1D1"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -746,8 +745,8 @@
   </sheetPr>
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -947,7 +946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="n">
         <v>30</v>
       </c>
@@ -992,7 +991,7 @@
       <c r="D16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1009,7 +1008,7 @@
       <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1026,7 +1025,7 @@
       <c r="D18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1043,7 +1042,7 @@
       <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>47</v>
       </c>
       <c r="G19" s="3"/>
@@ -1058,10 +1057,10 @@
       <c r="C20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1101,14 +1100,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="n">
         <v>12</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -1117,7 +1116,7 @@
       <c r="E23" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>62</v>
       </c>
       <c r="G23" s="0"/>
@@ -1129,25 +1128,25 @@
       <c r="B24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>64</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E24" s="0"/>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="n">
         <v>20</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -1156,55 +1155,55 @@
       <c r="E25" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="15" t="s">
         <v>71</v>
       </c>
       <c r="G25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="n">
+      <c r="A26" s="16" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="n">
+      <c r="A27" s="16" t="n">
         <v>18</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="16"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="n">
+      <c r="A28" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="16"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="n">
@@ -1213,143 +1212,149 @@
       <c r="B29" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>79</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E29" s="0"/>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="n">
+      <c r="A30" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="16"/>
+      <c r="E30" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
+      <c r="A31" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="C31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="16"/>
+      <c r="E31" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="n">
+      <c r="A32" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="15" t="s">
+      <c r="B32" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F32" s="24"/>
+        <v>89</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23" t="n">
+      <c r="A33" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="B33" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="B33" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" s="24"/>
+        <v>92</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="n">
         <v>14</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>98</v>
       </c>
       <c r="G34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="n">
+      <c r="A35" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="18" t="s">
+      <c r="B35" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="16"/>
+      <c r="D35" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="n">
         <v>24</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="16"/>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="n">
         <v>25</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>15</v>
@@ -1360,16 +1365,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="14" t="s">
-        <v>102</v>
+      <c r="E38" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,52 +1382,52 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="14" t="s">
         <v>50</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="n">
+      <c r="A40" s="22" t="n">
         <v>40</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="15" t="s">
+      <c r="B40" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>88</v>
+        <v>110</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="F40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="n">
+      <c r="A41" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="15" t="s">
+      <c r="B41" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>88</v>
+        <v>113</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="F41" s="0"/>
     </row>
@@ -1430,189 +1435,189 @@
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>88</v>
+      <c r="A43" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="F43" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G45" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="H45" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="I45" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="J45" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="K45" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="L45" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="M45" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="N45" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="O45" s="28" t="s">
+      <c r="G45" s="24" t="s">
         <v>120</v>
       </c>
+      <c r="H45" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="K45" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="L45" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="M45" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="N45" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="O45" s="24" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="29" t="n">
+      <c r="H46" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I46" s="29" t="n">
+      <c r="I46" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="J46" s="29" t="n">
+      <c r="J46" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K46" s="29" t="n">
+      <c r="K46" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="L46" s="29" t="n">
+      <c r="L46" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="M46" s="29" t="n">
+      <c r="M46" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="N46" s="29" t="n">
+      <c r="N46" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="O46" s="29" t="n">
+      <c r="O46" s="25" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G47" s="29" t="n">
+      <c r="G47" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="30"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="30"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-      <c r="M50" s="30"/>
-      <c r="N50" s="30"/>
-      <c r="O50" s="30"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
-      <c r="L52" s="30"/>
-      <c r="M52" s="30"/>
-      <c r="N52" s="30"/>
-      <c r="O52" s="30"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
-      <c r="L53" s="30"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="30"/>
-      <c r="O53" s="30"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="30"/>
-      <c r="M54" s="30"/>
-      <c r="N54" s="30"/>
-      <c r="O54" s="30"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="30"/>
-      <c r="O55" s="30"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="30"/>
-      <c r="L56" s="30"/>
-      <c r="M56" s="30"/>
-      <c r="N56" s="30"/>
-      <c r="O56" s="30"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G57" s="0"/>
@@ -1627,7 +1632,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J58" s="2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>